<commit_message>
changed start date of currency regression test
</commit_message>
<xml_diff>
--- a/UPDATED YOUTROOPERS schedule.xlsx
+++ b/UPDATED YOUTROOPERS schedule.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Clarice Alyson Ho\Downloads\Telegram Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\smutroopers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{656F49E3-A559-4791-8FA6-BDA17A36B850}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8B7F6AA-681F-48B9-B5AF-EF29271CF49C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3129,6 +3129,28 @@
     <xf numFmtId="0" fontId="71" fillId="33" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="48" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="48" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="48" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="41" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="41" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="41" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="41" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="14" fontId="70" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
@@ -3136,29 +3158,7 @@
     <xf numFmtId="0" fontId="54" fillId="0" borderId="0" xfId="34" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="48" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="48" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="48" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="164" fontId="41" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="167" fontId="41" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="41" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="41" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="41" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
       <protection locked="0"/>
     </xf>
@@ -3917,8 +3917,8 @@
   <dimension ref="A1:BN62"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="68" zoomScaleNormal="68" workbookViewId="0">
-      <pane ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G44" sqref="G44"/>
+      <pane ySplit="7" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H43" sqref="H43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -3948,27 +3948,27 @@
       <c r="F1" s="37"/>
       <c r="G1" s="37"/>
       <c r="J1" s="70"/>
-      <c r="K1" s="182"/>
-      <c r="L1" s="182"/>
-      <c r="M1" s="182"/>
-      <c r="N1" s="182"/>
-      <c r="O1" s="182"/>
-      <c r="P1" s="182"/>
-      <c r="Q1" s="182"/>
-      <c r="R1" s="182"/>
-      <c r="S1" s="182"/>
-      <c r="T1" s="182"/>
-      <c r="U1" s="182"/>
-      <c r="V1" s="182"/>
-      <c r="W1" s="182"/>
-      <c r="X1" s="182"/>
-      <c r="Y1" s="182"/>
-      <c r="Z1" s="182"/>
-      <c r="AA1" s="182"/>
-      <c r="AB1" s="182"/>
-      <c r="AC1" s="182"/>
-      <c r="AD1" s="182"/>
-      <c r="AE1" s="182"/>
+      <c r="K1" s="189"/>
+      <c r="L1" s="189"/>
+      <c r="M1" s="189"/>
+      <c r="N1" s="189"/>
+      <c r="O1" s="189"/>
+      <c r="P1" s="189"/>
+      <c r="Q1" s="189"/>
+      <c r="R1" s="189"/>
+      <c r="S1" s="189"/>
+      <c r="T1" s="189"/>
+      <c r="U1" s="189"/>
+      <c r="V1" s="189"/>
+      <c r="W1" s="189"/>
+      <c r="X1" s="189"/>
+      <c r="Y1" s="189"/>
+      <c r="Z1" s="189"/>
+      <c r="AA1" s="189"/>
+      <c r="AB1" s="189"/>
+      <c r="AC1" s="189"/>
+      <c r="AD1" s="189"/>
+      <c r="AE1" s="189"/>
     </row>
     <row r="2" spans="1:66" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="41" t="s">
@@ -3983,11 +3983,11 @@
       <c r="I2" s="2"/>
     </row>
     <row r="3" spans="1:66" ht="14" x14ac:dyDescent="0.25">
-      <c r="A3" s="181">
+      <c r="A3" s="188">
         <f ca="1">TODAY()</f>
         <v>43853</v>
       </c>
-      <c r="B3" s="181"/>
+      <c r="B3" s="188"/>
       <c r="C3" s="160"/>
       <c r="D3" s="151"/>
       <c r="E3" s="4"/>
@@ -4019,11 +4019,11 @@
         <v>41</v>
       </c>
       <c r="C4" s="161"/>
-      <c r="D4" s="186">
+      <c r="D4" s="190">
         <v>43703</v>
       </c>
-      <c r="E4" s="186"/>
-      <c r="F4" s="186"/>
+      <c r="E4" s="190"/>
+      <c r="F4" s="190"/>
       <c r="G4" s="60"/>
       <c r="H4" s="63" t="s">
         <v>40</v>
@@ -4032,182 +4032,182 @@
         <v>12</v>
       </c>
       <c r="J4" s="61"/>
-      <c r="K4" s="183" t="str">
+      <c r="K4" s="181" t="str">
         <f>"Week "&amp;(K6-($D$4-WEEKDAY($D$4,1)+2))/7+1</f>
         <v>Week 12</v>
       </c>
-      <c r="L4" s="184"/>
-      <c r="M4" s="184"/>
-      <c r="N4" s="184"/>
-      <c r="O4" s="184"/>
-      <c r="P4" s="184"/>
-      <c r="Q4" s="185"/>
-      <c r="R4" s="183" t="str">
+      <c r="L4" s="182"/>
+      <c r="M4" s="182"/>
+      <c r="N4" s="182"/>
+      <c r="O4" s="182"/>
+      <c r="P4" s="182"/>
+      <c r="Q4" s="183"/>
+      <c r="R4" s="181" t="str">
         <f>"Week "&amp;(R6-($D$4-WEEKDAY($D$4,1)+2))/7+1</f>
         <v>Week 13</v>
       </c>
-      <c r="S4" s="184"/>
-      <c r="T4" s="184"/>
-      <c r="U4" s="184"/>
-      <c r="V4" s="184"/>
-      <c r="W4" s="184"/>
-      <c r="X4" s="185"/>
-      <c r="Y4" s="183" t="str">
+      <c r="S4" s="182"/>
+      <c r="T4" s="182"/>
+      <c r="U4" s="182"/>
+      <c r="V4" s="182"/>
+      <c r="W4" s="182"/>
+      <c r="X4" s="183"/>
+      <c r="Y4" s="181" t="str">
         <f>"Week "&amp;(Y6-($D$4-WEEKDAY($D$4,1)+2))/7+1</f>
         <v>Week 14</v>
       </c>
-      <c r="Z4" s="184"/>
-      <c r="AA4" s="184"/>
-      <c r="AB4" s="184"/>
-      <c r="AC4" s="184"/>
-      <c r="AD4" s="184"/>
-      <c r="AE4" s="185"/>
-      <c r="AF4" s="183" t="str">
+      <c r="Z4" s="182"/>
+      <c r="AA4" s="182"/>
+      <c r="AB4" s="182"/>
+      <c r="AC4" s="182"/>
+      <c r="AD4" s="182"/>
+      <c r="AE4" s="183"/>
+      <c r="AF4" s="181" t="str">
         <f>"Week "&amp;(AF6-($D$4-WEEKDAY($D$4,1)+2))/7+1</f>
         <v>Week 15</v>
       </c>
-      <c r="AG4" s="184"/>
-      <c r="AH4" s="184"/>
-      <c r="AI4" s="184"/>
-      <c r="AJ4" s="184"/>
-      <c r="AK4" s="184"/>
-      <c r="AL4" s="185"/>
-      <c r="AM4" s="183" t="str">
+      <c r="AG4" s="182"/>
+      <c r="AH4" s="182"/>
+      <c r="AI4" s="182"/>
+      <c r="AJ4" s="182"/>
+      <c r="AK4" s="182"/>
+      <c r="AL4" s="183"/>
+      <c r="AM4" s="181" t="str">
         <f>"Week "&amp;(AM6-($D$4-WEEKDAY($D$4,1)+2))/7+1</f>
         <v>Week 16</v>
       </c>
-      <c r="AN4" s="184"/>
-      <c r="AO4" s="184"/>
-      <c r="AP4" s="184"/>
-      <c r="AQ4" s="184"/>
-      <c r="AR4" s="184"/>
-      <c r="AS4" s="185"/>
-      <c r="AT4" s="183" t="str">
+      <c r="AN4" s="182"/>
+      <c r="AO4" s="182"/>
+      <c r="AP4" s="182"/>
+      <c r="AQ4" s="182"/>
+      <c r="AR4" s="182"/>
+      <c r="AS4" s="183"/>
+      <c r="AT4" s="181" t="str">
         <f>"Week "&amp;(AT6-($D$4-WEEKDAY($D$4,1)+2))/7+1</f>
         <v>Week 17</v>
       </c>
-      <c r="AU4" s="184"/>
-      <c r="AV4" s="184"/>
-      <c r="AW4" s="184"/>
-      <c r="AX4" s="184"/>
-      <c r="AY4" s="184"/>
-      <c r="AZ4" s="185"/>
-      <c r="BA4" s="183" t="str">
+      <c r="AU4" s="182"/>
+      <c r="AV4" s="182"/>
+      <c r="AW4" s="182"/>
+      <c r="AX4" s="182"/>
+      <c r="AY4" s="182"/>
+      <c r="AZ4" s="183"/>
+      <c r="BA4" s="181" t="str">
         <f>"Week "&amp;(BA6-($D$4-WEEKDAY($D$4,1)+2))/7+1</f>
         <v>Week 18</v>
       </c>
-      <c r="BB4" s="184"/>
-      <c r="BC4" s="184"/>
-      <c r="BD4" s="184"/>
-      <c r="BE4" s="184"/>
-      <c r="BF4" s="184"/>
-      <c r="BG4" s="185"/>
-      <c r="BH4" s="183" t="str">
+      <c r="BB4" s="182"/>
+      <c r="BC4" s="182"/>
+      <c r="BD4" s="182"/>
+      <c r="BE4" s="182"/>
+      <c r="BF4" s="182"/>
+      <c r="BG4" s="183"/>
+      <c r="BH4" s="181" t="str">
         <f>"Week "&amp;(BH6-($D$4-WEEKDAY($D$4,1)+2))/7+1</f>
         <v>Week 19</v>
       </c>
-      <c r="BI4" s="184"/>
-      <c r="BJ4" s="184"/>
-      <c r="BK4" s="184"/>
-      <c r="BL4" s="184"/>
-      <c r="BM4" s="184"/>
-      <c r="BN4" s="185"/>
+      <c r="BI4" s="182"/>
+      <c r="BJ4" s="182"/>
+      <c r="BK4" s="182"/>
+      <c r="BL4" s="182"/>
+      <c r="BM4" s="182"/>
+      <c r="BN4" s="183"/>
     </row>
     <row r="5" spans="1:66" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="59"/>
       <c r="B5" s="63" t="s">
         <v>111</v>
       </c>
-      <c r="C5" s="190" t="s">
+      <c r="C5" s="187" t="s">
         <v>112</v>
       </c>
-      <c r="D5" s="190"/>
-      <c r="E5" s="190"/>
-      <c r="F5" s="190"/>
-      <c r="G5" s="190"/>
+      <c r="D5" s="187"/>
+      <c r="E5" s="187"/>
+      <c r="F5" s="187"/>
+      <c r="G5" s="187"/>
       <c r="H5" s="62"/>
       <c r="I5" s="62"/>
       <c r="J5" s="62"/>
-      <c r="K5" s="187">
+      <c r="K5" s="184">
         <f>K6</f>
         <v>43780</v>
       </c>
-      <c r="L5" s="188"/>
-      <c r="M5" s="188"/>
-      <c r="N5" s="188"/>
-      <c r="O5" s="188"/>
-      <c r="P5" s="188"/>
-      <c r="Q5" s="189"/>
-      <c r="R5" s="187">
+      <c r="L5" s="185"/>
+      <c r="M5" s="185"/>
+      <c r="N5" s="185"/>
+      <c r="O5" s="185"/>
+      <c r="P5" s="185"/>
+      <c r="Q5" s="186"/>
+      <c r="R5" s="184">
         <f>R6</f>
         <v>43787</v>
       </c>
-      <c r="S5" s="188"/>
-      <c r="T5" s="188"/>
-      <c r="U5" s="188"/>
-      <c r="V5" s="188"/>
-      <c r="W5" s="188"/>
-      <c r="X5" s="189"/>
-      <c r="Y5" s="187">
+      <c r="S5" s="185"/>
+      <c r="T5" s="185"/>
+      <c r="U5" s="185"/>
+      <c r="V5" s="185"/>
+      <c r="W5" s="185"/>
+      <c r="X5" s="186"/>
+      <c r="Y5" s="184">
         <f>Y6</f>
         <v>43794</v>
       </c>
-      <c r="Z5" s="188"/>
-      <c r="AA5" s="188"/>
-      <c r="AB5" s="188"/>
-      <c r="AC5" s="188"/>
-      <c r="AD5" s="188"/>
-      <c r="AE5" s="189"/>
-      <c r="AF5" s="187">
+      <c r="Z5" s="185"/>
+      <c r="AA5" s="185"/>
+      <c r="AB5" s="185"/>
+      <c r="AC5" s="185"/>
+      <c r="AD5" s="185"/>
+      <c r="AE5" s="186"/>
+      <c r="AF5" s="184">
         <f>AF6</f>
         <v>43801</v>
       </c>
-      <c r="AG5" s="188"/>
-      <c r="AH5" s="188"/>
-      <c r="AI5" s="188"/>
-      <c r="AJ5" s="188"/>
-      <c r="AK5" s="188"/>
-      <c r="AL5" s="189"/>
-      <c r="AM5" s="187">
+      <c r="AG5" s="185"/>
+      <c r="AH5" s="185"/>
+      <c r="AI5" s="185"/>
+      <c r="AJ5" s="185"/>
+      <c r="AK5" s="185"/>
+      <c r="AL5" s="186"/>
+      <c r="AM5" s="184">
         <f>AM6</f>
         <v>43808</v>
       </c>
-      <c r="AN5" s="188"/>
-      <c r="AO5" s="188"/>
-      <c r="AP5" s="188"/>
-      <c r="AQ5" s="188"/>
-      <c r="AR5" s="188"/>
-      <c r="AS5" s="189"/>
-      <c r="AT5" s="187">
+      <c r="AN5" s="185"/>
+      <c r="AO5" s="185"/>
+      <c r="AP5" s="185"/>
+      <c r="AQ5" s="185"/>
+      <c r="AR5" s="185"/>
+      <c r="AS5" s="186"/>
+      <c r="AT5" s="184">
         <f>AT6</f>
         <v>43815</v>
       </c>
-      <c r="AU5" s="188"/>
-      <c r="AV5" s="188"/>
-      <c r="AW5" s="188"/>
-      <c r="AX5" s="188"/>
-      <c r="AY5" s="188"/>
-      <c r="AZ5" s="189"/>
-      <c r="BA5" s="187">
+      <c r="AU5" s="185"/>
+      <c r="AV5" s="185"/>
+      <c r="AW5" s="185"/>
+      <c r="AX5" s="185"/>
+      <c r="AY5" s="185"/>
+      <c r="AZ5" s="186"/>
+      <c r="BA5" s="184">
         <f>BA6</f>
         <v>43822</v>
       </c>
-      <c r="BB5" s="188"/>
-      <c r="BC5" s="188"/>
-      <c r="BD5" s="188"/>
-      <c r="BE5" s="188"/>
-      <c r="BF5" s="188"/>
-      <c r="BG5" s="189"/>
-      <c r="BH5" s="187">
+      <c r="BB5" s="185"/>
+      <c r="BC5" s="185"/>
+      <c r="BD5" s="185"/>
+      <c r="BE5" s="185"/>
+      <c r="BF5" s="185"/>
+      <c r="BG5" s="186"/>
+      <c r="BH5" s="184">
         <f>BH6</f>
         <v>43829</v>
       </c>
-      <c r="BI5" s="188"/>
-      <c r="BJ5" s="188"/>
-      <c r="BK5" s="188"/>
-      <c r="BL5" s="188"/>
-      <c r="BM5" s="188"/>
-      <c r="BN5" s="189"/>
+      <c r="BI5" s="185"/>
+      <c r="BJ5" s="185"/>
+      <c r="BK5" s="185"/>
+      <c r="BL5" s="185"/>
+      <c r="BM5" s="185"/>
+      <c r="BN5" s="186"/>
     </row>
     <row r="6" spans="1:66" x14ac:dyDescent="0.25">
       <c r="A6" s="38"/>
@@ -7659,7 +7659,7 @@
         <v>5.0999999999999996</v>
       </c>
       <c r="F43" s="166">
-        <v>43867</v>
+        <v>43852</v>
       </c>
       <c r="G43" s="178">
         <v>43874</v>
@@ -9129,6 +9129,16 @@
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertRows="0" deleteRows="0"/>
   <mergeCells count="20">
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="K1:AE1"/>
+    <mergeCell ref="R4:X4"/>
+    <mergeCell ref="K4:Q4"/>
+    <mergeCell ref="D4:F4"/>
+    <mergeCell ref="R5:X5"/>
+    <mergeCell ref="K5:Q5"/>
+    <mergeCell ref="Y4:AE4"/>
+    <mergeCell ref="Y5:AE5"/>
+    <mergeCell ref="C5:G5"/>
     <mergeCell ref="AF4:AL4"/>
     <mergeCell ref="AF5:AL5"/>
     <mergeCell ref="BH4:BN4"/>
@@ -9139,16 +9149,6 @@
     <mergeCell ref="AM4:AS4"/>
     <mergeCell ref="BA4:BG4"/>
     <mergeCell ref="BA5:BG5"/>
-    <mergeCell ref="R5:X5"/>
-    <mergeCell ref="K5:Q5"/>
-    <mergeCell ref="Y4:AE4"/>
-    <mergeCell ref="Y5:AE5"/>
-    <mergeCell ref="C5:G5"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="K1:AE1"/>
-    <mergeCell ref="R4:X4"/>
-    <mergeCell ref="K4:Q4"/>
-    <mergeCell ref="D4:F4"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="I8:I11 I31:I43 I29 I45:I61 I13:I20">

</xml_diff>